<commit_message>
Final Update With Comments
</commit_message>
<xml_diff>
--- a/Semantic_Analysis/Result/Document_vs_Document_Similarity/Document_vs_Document_Similarity_Result.xlsx
+++ b/Semantic_Analysis/Result/Document_vs_Document_Similarity/Document_vs_Document_Similarity_Result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amman\Desktop\Result\Document_Similarity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Master_Of_Engg_IT\SE Project\Aman-Patel\semantic-analysis\Semantic_Analysis\Result\Document_vs_Document_Similarity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0570EB7B-6D34-4E05-BDAB-74867529F0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC89B8D-6110-4BC9-9485-CCC8E305E494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,10 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Reference Document 
-Machine Learning</t>
-  </si>
-  <si>
     <t xml:space="preserve">Water Pollution </t>
   </si>
   <si>
@@ -38,6 +34,10 @@
   </si>
   <si>
     <t>Documents</t>
+  </si>
+  <si>
+    <t>Reference Document 
+(Machine Learning)</t>
   </si>
 </sst>
 </file>
@@ -61,7 +61,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -69,18 +69,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -133,8 +149,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Machine Learning</a:t>
+              <a:t>Documents</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Reference Document (text-embedding-3-large)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -187,6 +208,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-9087-4765-B735-BD81F764D328}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1002,9 +1044,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1298,7 +1340,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1309,26 +1351,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>0.356727952971997</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.58031977841148097</v>
       </c>
     </row>

</xml_diff>